<commit_message>
updated module list, again
</commit_message>
<xml_diff>
--- a/data/17_cluster/config.xlsx
+++ b/data/17_cluster/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/6998A4BA-FB15-44D1-A6AD-18AE17E78A6F/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/stress/data/17_cluster/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/15D28717-6353-4C08-B9FC-9D341E2B75B5/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/stress/data/17_cluster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F439106-ADFF-4745-951B-5A5E928FBC2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A01AAC-8C9B-CA4F-BA6C-E0425FE266D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="7280" windowWidth="10000" windowHeight="18820" xr2:uid="{D70F0D5F-63CF-AE44-9328-5C6897092FCC}"/>
+    <workbookView xWindow="15920" yWindow="2180" windowWidth="10000" windowHeight="18820" xr2:uid="{D70F0D5F-63CF-AE44-9328-5C6897092FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="picked" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="310">
   <si>
     <t>cid</t>
   </si>
@@ -957,7 +957,7 @@
     <t>idx</t>
   </si>
   <si>
-    <t>transient activation (1h)</t>
+    <t>early repreession</t>
   </si>
 </sst>
 </file>
@@ -1405,10 +1405,10 @@
         <v>190</v>
       </c>
       <c r="C2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" t="s">
-        <v>232</v>
+        <v>167</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,10 +1419,10 @@
         <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" t="s">
-        <v>200</v>
+        <v>172</v>
+      </c>
+      <c r="D3">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1432,12 +1432,6 @@
       <c r="B4" t="s">
         <v>192</v>
       </c>
-      <c r="C4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" t="s">
-        <v>233</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1447,10 +1441,10 @@
         <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D5" t="s">
-        <v>201</v>
+        <v>171</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1460,6 +1454,12 @@
       <c r="B6" t="s">
         <v>194</v>
       </c>
+      <c r="C6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1589,10 +1589,10 @@
         <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" t="s">
-        <v>242</v>
+        <v>188</v>
+      </c>
+      <c r="D22">
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1603,10 +1603,10 @@
         <v>211</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
-      </c>
-      <c r="D23" t="s">
-        <v>244</v>
+        <v>309</v>
+      </c>
+      <c r="D23">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1616,12 +1616,6 @@
       <c r="B24" t="s">
         <v>212</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D24" t="s">
-        <v>243</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
@@ -1630,11 +1624,11 @@
       <c r="B25" t="s">
         <v>213</v>
       </c>
-      <c r="C25" t="s">
-        <v>175</v>
-      </c>
-      <c r="D25" t="s">
-        <v>252</v>
+      <c r="C25" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1643,12 +1637,6 @@
       </c>
       <c r="B26" t="s">
         <v>214</v>
-      </c>
-      <c r="C26" t="s">
-        <v>177</v>
-      </c>
-      <c r="D26" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>